<commit_message>
sizing with worst case
</commit_message>
<xml_diff>
--- a/Converters_Library.xlsx
+++ b/Converters_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c30483\Documents\dc_design_tool\dc_design_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8726F5E8-BB07-46F7-B53E-9DD1214C1EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D62F69-DB91-4726-A06D-0A26B59B96AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16410" windowWidth="29040" windowHeight="15720" xr2:uid="{B310722E-489A-462F-B946-DDE9E21437D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B310722E-489A-462F-B946-DDE9E21437D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Converters" sheetId="2" r:id="rId1"/>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE1DD91-E4BB-483E-AD34-9CF8C62E28B1}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I82" sqref="I82:I85"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3221,6 +3221,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005D48458B7DF5B44891BF6C8B708F036C" ma:contentTypeVersion="15" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="6ec72bf5cc41951886dd851de9b63939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a656bf76-cca4-4796-b3e3-9ff4debad9ca" xmlns:ns3="3f4d043c-ef99-408b-9086-307465b47223" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="619265aacb58e563d368a43a0aeb056e" ns2:_="" ns3:_="">
     <xsd:import namespace="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
@@ -3455,15 +3464,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4198C07A-8C8E-492A-A3EC-F4C24C93A879}">
   <ds:schemaRefs>
@@ -3476,6 +3476,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00F984FD-7FB1-4E24-9C54-AB8DB7C9EB67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F970F1C-4AA8-4790-8FBB-C76490AE23B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3492,12 +3500,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00F984FD-7FB1-4E24-9C54-AB8DB7C9EB67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
droop curve dc load
</commit_message>
<xml_diff>
--- a/Converters_Library.xlsx
+++ b/Converters_Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c30483\Documents\dc_design_tool\dc_design_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D62F69-DB91-4726-A06D-0A26B59B96AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8B5823-D5CD-4E55-B17F-A0699E99C848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B310722E-489A-462F-B946-DDE9E21437D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B310722E-489A-462F-B946-DDE9E21437D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Converters" sheetId="2" r:id="rId1"/>
@@ -618,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE1DD91-E4BB-483E-AD34-9CF8C62E28B1}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
       <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
@@ -3210,26 +3210,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a656bf76-cca4-4796-b3e3-9ff4debad9ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3f4d043c-ef99-408b-9086-307465b47223" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005D48458B7DF5B44891BF6C8B708F036C" ma:contentTypeVersion="15" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="6ec72bf5cc41951886dd851de9b63939">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a656bf76-cca4-4796-b3e3-9ff4debad9ca" xmlns:ns3="3f4d043c-ef99-408b-9086-307465b47223" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="619265aacb58e563d368a43a0aeb056e" ns2:_="" ns3:_="">
     <xsd:import namespace="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
@@ -3464,26 +3444,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4198C07A-8C8E-492A-A3EC-F4C24C93A879}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
-    <ds:schemaRef ds:uri="3f4d043c-ef99-408b-9086-307465b47223"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00F984FD-7FB1-4E24-9C54-AB8DB7C9EB67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a656bf76-cca4-4796-b3e3-9ff4debad9ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3f4d043c-ef99-408b-9086-307465b47223" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F970F1C-4AA8-4790-8FBB-C76490AE23B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3500,4 +3481,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00F984FD-7FB1-4E24-9C54-AB8DB7C9EB67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4198C07A-8C8E-492A-A3EC-F4C24C93A879}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a656bf76-cca4-4796-b3e3-9ff4debad9ca"/>
+    <ds:schemaRef ds:uri="3f4d043c-ef99-408b-9086-307465b47223"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>